<commit_message>
[DA] Refresh dev build with breadcrumb fixes and reference.xlsx for BCU
</commit_message>
<xml_diff>
--- a/tools/da-apps/dist/static/files/reference.xlsx
+++ b/tools/da-apps/dist/static/files/reference.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10420"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AAA624-7140-6B48-9BDE-FA2F242CD5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="900" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Report" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Invalid Pages" state="visible" r:id="rId5"/>
+    <sheet name="Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Invalid Pages" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>URL</t>
   </si>
@@ -59,158 +63,97 @@
     <t>URL_PATH</t>
   </si>
   <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>METAKEYINDEX</t>
-  </si>
-  <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t>KEYWORDS</t>
-  </si>
-  <si>
-    <t>SERP-CONTENT-TYPE</t>
-  </si>
-  <si>
-    <t>PUBLISHDATE</t>
-  </si>
-  <si>
-    <t>PRIMARYPRODUCTNAME</t>
-  </si>
-  <si>
-    <t>IMAGE</t>
-  </si>
-  <si>
-    <t>https://main--bacom--adobecom.hlx.page/index.md</t>
-  </si>
-  <si>
-    <t>https://main--bacom--adobecom.hlx.page</t>
+    <t>META_JSON</t>
+  </si>
+  <si>
+    <t>https://main--da-bacom--adobecom.aem.page/drafts/dshet/finalfolder/finalpage1.md</t>
+  </si>
+  <si>
+    <t>https://main--da-bacom--adobecom.aem.page</t>
   </si>
   <si>
     <t>us</t>
   </si>
   <si>
-    <t>index.md</t>
-  </si>
-  <si>
-    <t>mdast.children[51].children[0]</t>
-  </si>
-  <si>
-    <t>[51,0]</t>
-  </si>
-  <si>
-    <t>metadata</t>
-  </si>
-  <si>
-    <t>{"type":"gtBody","children":[{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"strong","children":[{"type":"text","value":"Metadata"}]}]}],"colSpan":2}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Title"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Adobe for Business | Enterprise Digital Marketing\nSolutions"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Description"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Drive growth and engage customers across channels with\npersonalized experiences from Adobe's powerful digital\nmarketing, analytics, commerce, AI, and automation tools."}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"keywords"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"adobe business, adobe for business, adobe marketing,\nadobe digital experience"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"serp-content-type"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"product"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"publishDate"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"2023-06-27"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"primaryProductName"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"All DX"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"image"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"image","alt":"Gradient color Adobe brand logo","label":"image10","url":"https://main--bacom--adobecom.hlx.page/media_17c6ba459a3827753e7830e7f91cc5c8eee4c2caf.jpeg#width=756&amp;height=426"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Footer-source"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"link","title":null,"url":"https://main--bacom--adobecom.hlx.page/footer","children":[{"type":"text","value":"https://main--bacom--adobecom.hlx.page/footer"}]}]}]}]}]}</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>{"blockType":"metadata","blockName":"metadata","keys":[]}</t>
-  </si>
-  <si>
-    <t>globalReturn</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/api/block/getMdast?url=https://main--bacom--adobecom.hlx.page/index.md&amp;path=mdast.children[51].children[0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adobe for Business | Enterprise Digital Marketing
-Solutions</t>
-  </si>
-  <si>
-    <t>0,8,1,0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drive growth and engage customers across channels with
-personalized experiences from Adobe's powerful digital
-marketing, analytics, commerce, AI, and automation tools.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adobe business, adobe for business, adobe marketing,
-adobe digital experience</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>2023-06-27</t>
-  </si>
-  <si>
-    <t>All DX</t>
-  </si>
-  <si>
-    <t>https://main--bacom--adobecom.hlx.page/media_17c6ba459a3827753e7830e7f91cc5c8eee4c2caf.jpeg#width=756&amp;height=426</t>
-  </si>
-  <si>
-    <t>https://main--bacom--adobecom.hlx.page/ca/index.md</t>
-  </si>
-  <si>
-    <t>ca</t>
-  </si>
-  <si>
-    <t>mdast.children[53].children[0]</t>
-  </si>
-  <si>
-    <t>[53,0]</t>
-  </si>
-  <si>
-    <t>{"type":"gtBody","children":[{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"strong","children":[{"type":"text","value":"Metadata"}]}]}],"colSpan":2}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Title"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Adobe for Business | Enterprise Digital Marketing\nSolutions"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Description"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Drive growth and engage customers across channels with\npersonalized experiences from Adobe's powerful digital\nmarketing, analytics, commerce, AI, and automation tools."}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"keywords"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"adobe business, adobe for business, adobe marketing,\nadobe digital experience"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"serp-content-type"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"product"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"publishDate"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"2023-06-27"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"primaryProductName"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"All DX"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"image"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"image","alt":"Gradient color Adobe brand logo","label":"image16","url":"https://main--bacom--adobecom.hlx.page/media_17c6ba459a3827753e7830e7f91cc5c8eee4c2caf.jpeg#width=756&amp;height=426"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Footer-source"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"link","title":null,"url":"https://main--bacom--adobecom.hlx.page/footer","children":[{"type":"text","value":"https://main--bacom--adobecom.hlx.page/footer"}]}]}]}]}]}</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/api/block/getMdast?url=https://main--bacom--adobecom.hlx.page/ca/index.md&amp;path=mdast.children[53].children[0]</t>
-  </si>
-  <si>
-    <t>https://main--bacom--adobecom.hlx.page/ca_fr/index.md</t>
-  </si>
-  <si>
-    <t>ca_fr</t>
-  </si>
-  <si>
-    <t>mdast.children[56].children[0]</t>
-  </si>
-  <si>
-    <t>[56,0]</t>
-  </si>
-  <si>
-    <t>{"type":"gtBody","children":[{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Metadata"}]}],"colSpan":2}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Title"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Adobe for Business | Solutions de marketing numérique\npour les entreprises"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Description"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Déployez des expériences personnalisées et attrayantes sur\ntous les canaux. Stimulez ainsi votre croissance grâce aux\npuissantes solutions d'Adobe pour le marketing numérique,\nl'analytique, le commerce, l'IA et l'automatisation."}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"keywords"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Adobe Business, Adobe for Business, solutions marketing\nAdobe, solutions d'expérience numérique Adobe"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"serp-content-type"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"product"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"publishDate"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"2023-06-27"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"primaryProductName"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"All DX"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"image"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"image","alt":"Logo de la marque Adobe en dégradé de couleurs","label":"image16","url":"https://main--bacom--adobecom.hlx.page/media_17c6ba459a3827753e7830e7f91cc5c8eee4c2caf.jpeg#width=756&amp;height=426"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Footer-source"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"link","title":null,"url":"https://main--bacom--adobecom.hlx.page/footer","children":[{"type":"text","value":"https://main--bacom--adobecom.hlx.page/footer"}]}]}]}]}]}</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/api/block/getMdast?url=https://main--bacom--adobecom.hlx.page/ca_fr/index.md&amp;path=mdast.children[56].children[0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adobe for Business | Solutions de marketing numérique
-pour les entreprises</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Déployez des expériences personnalisées et attrayantes sur
-tous les canaux. Stimulez ainsi votre croissance grâce aux
-puissantes solutions d'Adobe pour le marketing numérique,
-l'analytique, le commerce, l'IA et l'automatisation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adobe Business, Adobe for Business, solutions marketing
-Adobe, solutions d'expérience numérique Adobe</t>
+    <t>drafts/dshet/finalfolder/finalpage1.md</t>
+  </si>
+  <si>
+    <t>mdast.children[1].children[0].children[1].children[0].children[2]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,2]</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>text (long form, large)</t>
+  </si>
+  <si>
+    <t>{"type":"paragraph","children":[{"type":"text","value":"White jasmin flower"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White jasmin flower
+</t>
+  </si>
+  <si>
+    <t>White jasmin flower</t>
+  </si>
+  <si>
+    <t>{"operation":"LIKE","searchValue":"White jasmin flower"}</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/block/getMdast?url=https://main--da-bacom--adobecom.aem.page/drafts/dshet/finalfolder/finalpage1.md&amp;path=mdast.children[1].children[0].children[1].children[0].children[2]</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>https://main--da-bacom--adobecom.aem.page/drafts/dshet/finalfolder/finalpage2.md</t>
+  </si>
+  <si>
+    <t>drafts/dshet/finalfolder/finalpage2.md</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/block/getMdast?url=https://main--da-bacom--adobecom.aem.page/drafts/dshet/finalfolder/finalpage2.md&amp;path=mdast.children[1].children[0].children[1].children[0].children[2]</t>
   </si>
   <si>
     <t>STATUS</t>
+  </si>
+  <si>
+    <t>UPDATE_MD_DATA</t>
+  </si>
+  <si>
+    <t>OPERATION_TYPE</t>
+  </si>
+  <si>
+    <t>replace</t>
+  </si>
+  <si>
+    <t>UPDATE_TYPE</t>
+  </si>
+  <si>
+    <t>md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pink jasmin flower
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -233,8 +176,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,17 +519,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="50" customWidth="1"/>
+    <col min="1" max="1" width="80.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="80" customWidth="1"/>
@@ -593,10 +542,13 @@
     <col min="11" max="11" width="20" customWidth="1"/>
     <col min="12" max="12" width="30" customWidth="1"/>
     <col min="13" max="13" width="50" customWidth="1"/>
-    <col min="14" max="23" width="30" customWidth="1"/>
+    <col min="14" max="16" width="30" customWidth="1"/>
+    <col min="17" max="17" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -646,271 +598,166 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="M2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="N2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
+      <c r="O2" t="s">
         <v>29</v>
       </c>
-      <c r="H2">
-        <v>51</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
         <v>30</v>
       </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
+      <c r="Q2" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="R2" t="s">
         <v>37</v>
       </c>
       <c r="S2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" t="s">
         <v>39</v>
       </c>
-      <c r="U2" t="s">
+    </row>
+    <row r="3" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="V2" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3">
-        <v>53</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>36</v>
       </c>
       <c r="R3" t="s">
         <v>37</v>
       </c>
       <c r="S3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" t="s">
         <v>39</v>
-      </c>
-      <c r="U3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4">
-        <v>56</v>
-      </c>
-      <c r="I4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" t="s">
-        <v>33</v>
-      </c>
-      <c r="O4" t="s">
-        <v>54</v>
-      </c>
-      <c r="P4" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" t="s">
-        <v>56</v>
-      </c>
-      <c r="S4" t="s">
-        <v>57</v>
-      </c>
-      <c r="T4" t="s">
-        <v>39</v>
-      </c>
-      <c r="U4" t="s">
-        <v>40</v>
-      </c>
-      <c r="V4" t="s">
-        <v>41</v>
-      </c>
-      <c r="W4" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[DA] Refresh dev build with breadcrumb fixes and reference.xlsx for BCU (#4086)
</commit_message>
<xml_diff>
--- a/tools/da-apps/dist/static/files/reference.xlsx
+++ b/tools/da-apps/dist/static/files/reference.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10420"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AAA624-7140-6B48-9BDE-FA2F242CD5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="900" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Report" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Invalid Pages" state="visible" r:id="rId5"/>
+    <sheet name="Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Invalid Pages" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>URL</t>
   </si>
@@ -59,158 +63,97 @@
     <t>URL_PATH</t>
   </si>
   <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>METAKEYINDEX</t>
-  </si>
-  <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t>KEYWORDS</t>
-  </si>
-  <si>
-    <t>SERP-CONTENT-TYPE</t>
-  </si>
-  <si>
-    <t>PUBLISHDATE</t>
-  </si>
-  <si>
-    <t>PRIMARYPRODUCTNAME</t>
-  </si>
-  <si>
-    <t>IMAGE</t>
-  </si>
-  <si>
-    <t>https://main--bacom--adobecom.hlx.page/index.md</t>
-  </si>
-  <si>
-    <t>https://main--bacom--adobecom.hlx.page</t>
+    <t>META_JSON</t>
+  </si>
+  <si>
+    <t>https://main--da-bacom--adobecom.aem.page/drafts/dshet/finalfolder/finalpage1.md</t>
+  </si>
+  <si>
+    <t>https://main--da-bacom--adobecom.aem.page</t>
   </si>
   <si>
     <t>us</t>
   </si>
   <si>
-    <t>index.md</t>
-  </si>
-  <si>
-    <t>mdast.children[51].children[0]</t>
-  </si>
-  <si>
-    <t>[51,0]</t>
-  </si>
-  <si>
-    <t>metadata</t>
-  </si>
-  <si>
-    <t>{"type":"gtBody","children":[{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"strong","children":[{"type":"text","value":"Metadata"}]}]}],"colSpan":2}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Title"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Adobe for Business | Enterprise Digital Marketing\nSolutions"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Description"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Drive growth and engage customers across channels with\npersonalized experiences from Adobe's powerful digital\nmarketing, analytics, commerce, AI, and automation tools."}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"keywords"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"adobe business, adobe for business, adobe marketing,\nadobe digital experience"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"serp-content-type"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"product"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"publishDate"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"2023-06-27"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"primaryProductName"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"All DX"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"image"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"image","alt":"Gradient color Adobe brand logo","label":"image10","url":"https://main--bacom--adobecom.hlx.page/media_17c6ba459a3827753e7830e7f91cc5c8eee4c2caf.jpeg#width=756&amp;height=426"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Footer-source"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"link","title":null,"url":"https://main--bacom--adobecom.hlx.page/footer","children":[{"type":"text","value":"https://main--bacom--adobecom.hlx.page/footer"}]}]}]}]}]}</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>{"blockType":"metadata","blockName":"metadata","keys":[]}</t>
-  </si>
-  <si>
-    <t>globalReturn</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/api/block/getMdast?url=https://main--bacom--adobecom.hlx.page/index.md&amp;path=mdast.children[51].children[0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adobe for Business | Enterprise Digital Marketing
-Solutions</t>
-  </si>
-  <si>
-    <t>0,8,1,0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drive growth and engage customers across channels with
-personalized experiences from Adobe's powerful digital
-marketing, analytics, commerce, AI, and automation tools.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adobe business, adobe for business, adobe marketing,
-adobe digital experience</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>2023-06-27</t>
-  </si>
-  <si>
-    <t>All DX</t>
-  </si>
-  <si>
-    <t>https://main--bacom--adobecom.hlx.page/media_17c6ba459a3827753e7830e7f91cc5c8eee4c2caf.jpeg#width=756&amp;height=426</t>
-  </si>
-  <si>
-    <t>https://main--bacom--adobecom.hlx.page/ca/index.md</t>
-  </si>
-  <si>
-    <t>ca</t>
-  </si>
-  <si>
-    <t>mdast.children[53].children[0]</t>
-  </si>
-  <si>
-    <t>[53,0]</t>
-  </si>
-  <si>
-    <t>{"type":"gtBody","children":[{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"strong","children":[{"type":"text","value":"Metadata"}]}]}],"colSpan":2}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Title"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Adobe for Business | Enterprise Digital Marketing\nSolutions"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Description"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Drive growth and engage customers across channels with\npersonalized experiences from Adobe's powerful digital\nmarketing, analytics, commerce, AI, and automation tools."}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"keywords"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"adobe business, adobe for business, adobe marketing,\nadobe digital experience"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"serp-content-type"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"product"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"publishDate"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"2023-06-27"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"primaryProductName"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"All DX"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"image"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"image","alt":"Gradient color Adobe brand logo","label":"image16","url":"https://main--bacom--adobecom.hlx.page/media_17c6ba459a3827753e7830e7f91cc5c8eee4c2caf.jpeg#width=756&amp;height=426"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Footer-source"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"link","title":null,"url":"https://main--bacom--adobecom.hlx.page/footer","children":[{"type":"text","value":"https://main--bacom--adobecom.hlx.page/footer"}]}]}]}]}]}</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/api/block/getMdast?url=https://main--bacom--adobecom.hlx.page/ca/index.md&amp;path=mdast.children[53].children[0]</t>
-  </si>
-  <si>
-    <t>https://main--bacom--adobecom.hlx.page/ca_fr/index.md</t>
-  </si>
-  <si>
-    <t>ca_fr</t>
-  </si>
-  <si>
-    <t>mdast.children[56].children[0]</t>
-  </si>
-  <si>
-    <t>[56,0]</t>
-  </si>
-  <si>
-    <t>{"type":"gtBody","children":[{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Metadata"}]}],"colSpan":2}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Title"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Adobe for Business | Solutions de marketing numérique\npour les entreprises"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Description"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Déployez des expériences personnalisées et attrayantes sur\ntous les canaux. Stimulez ainsi votre croissance grâce aux\npuissantes solutions d'Adobe pour le marketing numérique,\nl'analytique, le commerce, l'IA et l'automatisation."}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"keywords"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Adobe Business, Adobe for Business, solutions marketing\nAdobe, solutions d'expérience numérique Adobe"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"serp-content-type"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"product"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"publishDate"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"2023-06-27"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"primaryProductName"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"All DX"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"image"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"image","alt":"Logo de la marque Adobe en dégradé de couleurs","label":"image16","url":"https://main--bacom--adobecom.hlx.page/media_17c6ba459a3827753e7830e7f91cc5c8eee4c2caf.jpeg#width=756&amp;height=426"}]}]}]},{"type":"gtRow","children":[{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"text","value":"Footer-source"}]}]},{"type":"gtCell","children":[{"type":"paragraph","children":[{"type":"link","title":null,"url":"https://main--bacom--adobecom.hlx.page/footer","children":[{"type":"text","value":"https://main--bacom--adobecom.hlx.page/footer"}]}]}]}]}]}</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/api/block/getMdast?url=https://main--bacom--adobecom.hlx.page/ca_fr/index.md&amp;path=mdast.children[56].children[0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adobe for Business | Solutions de marketing numérique
-pour les entreprises</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Déployez des expériences personnalisées et attrayantes sur
-tous les canaux. Stimulez ainsi votre croissance grâce aux
-puissantes solutions d'Adobe pour le marketing numérique,
-l'analytique, le commerce, l'IA et l'automatisation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adobe Business, Adobe for Business, solutions marketing
-Adobe, solutions d'expérience numérique Adobe</t>
+    <t>drafts/dshet/finalfolder/finalpage1.md</t>
+  </si>
+  <si>
+    <t>mdast.children[1].children[0].children[1].children[0].children[2]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,2]</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>text (long form, large)</t>
+  </si>
+  <si>
+    <t>{"type":"paragraph","children":[{"type":"text","value":"White jasmin flower"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White jasmin flower
+</t>
+  </si>
+  <si>
+    <t>White jasmin flower</t>
+  </si>
+  <si>
+    <t>{"operation":"LIKE","searchValue":"White jasmin flower"}</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/block/getMdast?url=https://main--da-bacom--adobecom.aem.page/drafts/dshet/finalfolder/finalpage1.md&amp;path=mdast.children[1].children[0].children[1].children[0].children[2]</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>https://main--da-bacom--adobecom.aem.page/drafts/dshet/finalfolder/finalpage2.md</t>
+  </si>
+  <si>
+    <t>drafts/dshet/finalfolder/finalpage2.md</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/block/getMdast?url=https://main--da-bacom--adobecom.aem.page/drafts/dshet/finalfolder/finalpage2.md&amp;path=mdast.children[1].children[0].children[1].children[0].children[2]</t>
   </si>
   <si>
     <t>STATUS</t>
+  </si>
+  <si>
+    <t>UPDATE_MD_DATA</t>
+  </si>
+  <si>
+    <t>OPERATION_TYPE</t>
+  </si>
+  <si>
+    <t>replace</t>
+  </si>
+  <si>
+    <t>UPDATE_TYPE</t>
+  </si>
+  <si>
+    <t>md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pink jasmin flower
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -233,8 +176,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,17 +519,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="50" customWidth="1"/>
+    <col min="1" max="1" width="80.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="80" customWidth="1"/>
@@ -593,10 +542,13 @@
     <col min="11" max="11" width="20" customWidth="1"/>
     <col min="12" max="12" width="30" customWidth="1"/>
     <col min="13" max="13" width="50" customWidth="1"/>
-    <col min="14" max="23" width="30" customWidth="1"/>
+    <col min="14" max="16" width="30" customWidth="1"/>
+    <col min="17" max="17" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -646,271 +598,166 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="M2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="N2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
+      <c r="O2" t="s">
         <v>29</v>
       </c>
-      <c r="H2">
-        <v>51</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
         <v>30</v>
       </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
+      <c r="Q2" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="R2" t="s">
         <v>37</v>
       </c>
       <c r="S2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" t="s">
         <v>39</v>
       </c>
-      <c r="U2" t="s">
+    </row>
+    <row r="3" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="V2" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3">
-        <v>53</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>36</v>
       </c>
       <c r="R3" t="s">
         <v>37</v>
       </c>
       <c r="S3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" t="s">
         <v>39</v>
-      </c>
-      <c r="U3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4">
-        <v>56</v>
-      </c>
-      <c r="I4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" t="s">
-        <v>33</v>
-      </c>
-      <c r="O4" t="s">
-        <v>54</v>
-      </c>
-      <c r="P4" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" t="s">
-        <v>56</v>
-      </c>
-      <c r="S4" t="s">
-        <v>57</v>
-      </c>
-      <c r="T4" t="s">
-        <v>39</v>
-      </c>
-      <c r="U4" t="s">
-        <v>40</v>
-      </c>
-      <c r="V4" t="s">
-        <v>41</v>
-      </c>
-      <c r="W4" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>